<commit_message>
Major bug fix to include support for other languages, as the app stood before this there was no multi language support. Major changes had to be performed to various files.
</commit_message>
<xml_diff>
--- a/src/R/Modals/qarm_lang.xlsx
+++ b/src/R/Modals/qarm_lang.xlsx
@@ -377,7 +377,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>QA correcto</t>
+          <t>Controle de qualidade correto</t>
         </is>
       </c>
     </row>
@@ -389,7 +389,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>QA incorrecto</t>
+          <t>Controle de qualidade incorreto</t>
         </is>
       </c>
     </row>
@@ -401,7 +401,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>QA Reporte</t>
+          <t>Relatório de controle de qualidade</t>
         </is>
       </c>
     </row>
@@ -413,7 +413,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Descargar reporte</t>
+          <t>Baixar relatório</t>
         </is>
       </c>
     </row>
@@ -425,7 +425,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>El reporte de QA no ha encontrado errores en los datos.</t>
+          <t>O relatório de controle de qualidade não encontrou erros nos dados.</t>
         </is>
       </c>
     </row>
@@ -437,7 +437,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>El reporte de QA ha encontrado errores en los datos, revisar detalles en el informe de reporte.</t>
+          <t>O relatório de controle de qualidade encontrou erros nos dados. Revise os detalhes no relatório.</t>
         </is>
       </c>
     </row>
@@ -449,7 +449,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Configuración correcta</t>
+          <t>Configuração correta</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Configuración incorrecta</t>
+          <t>Configuração incorreta</t>
         </is>
       </c>
     </row>
@@ -473,7 +473,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Todos los paquetes fueron instalados</t>
+          <t>Todos os pacotes foram instalados</t>
         </is>
       </c>
     </row>
@@ -485,7 +485,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Algunos paquetes no fueron instalados:</t>
+          <t>Alguns pacotes não foram instalados:</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Cerrar</t>
+          <t>Fechar</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed data errors in reports.
</commit_message>
<xml_diff>
--- a/src/R/Modals/qarm_lang.xlsx
+++ b/src/R/Modals/qarm_lang.xlsx
@@ -377,7 +377,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Controle de qualidade correto</t>
+          <t>QA correcto</t>
         </is>
       </c>
     </row>
@@ -389,7 +389,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Controle de qualidade incorreto</t>
+          <t>QA incorrecto</t>
         </is>
       </c>
     </row>
@@ -401,7 +401,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Relatório de controle de qualidade</t>
+          <t>QA Reporte</t>
         </is>
       </c>
     </row>
@@ -413,7 +413,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Baixar relatório</t>
+          <t>Descargar reporte</t>
         </is>
       </c>
     </row>
@@ -425,7 +425,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>O relatório de controle de qualidade não encontrou erros nos dados.</t>
+          <t>El reporte de QA no ha encontrado errores en los datos.</t>
         </is>
       </c>
     </row>
@@ -437,7 +437,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>O relatório de controle de qualidade encontrou erros nos dados. Revise os detalhes no relatório.</t>
+          <t>El reporte de QA ha encontrado errores en los datos, revisar detalles en el informe de reporte.</t>
         </is>
       </c>
     </row>
@@ -449,7 +449,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Configuração correta</t>
+          <t>Configuración correcta</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Configuração incorreta</t>
+          <t>Configuración incorrecta</t>
         </is>
       </c>
     </row>
@@ -473,7 +473,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Todos os pacotes foram instalados</t>
+          <t>Todos los paquetes fueron instalados</t>
         </is>
       </c>
     </row>
@@ -485,7 +485,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Alguns pacotes não foram instalados:</t>
+          <t>Algunos paquetes no fueron instalados:</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Fechar</t>
+          <t>Cerrar</t>
         </is>
       </c>
     </row>

</xml_diff>